<commit_message>
Update Streamlit trip cost app with advanced FY26 per diem + YOS pay table
</commit_message>
<xml_diff>
--- a/MDEP Calculator.xlsx
+++ b/MDEP Calculator.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="82" documentId="11_F25DC773A252ABDACC104875615F5E0E5ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{93F008E4-13C3-4A29-9DD6-AE86683DF088}"/>
   <bookViews>
-    <workbookView xWindow="-28935" yWindow="-135" windowWidth="29070" windowHeight="15750" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27885" yWindow="2325" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -196,9 +196,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -211,11 +208,14 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -232,6 +232,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -500,1854 +504,1854 @@
   <dimension ref="A1:W26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10"/>
+      <selection activeCell="Q12" sqref="Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="23" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="6"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="1">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1">
         <v>4</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>6</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>8</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>10</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>12</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>14</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>16</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>18</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>20</v>
       </c>
-      <c r="N2" s="2">
+      <c r="N2" s="1">
         <v>22</v>
       </c>
-      <c r="O2" s="2">
+      <c r="O2" s="1">
         <v>24</v>
       </c>
-      <c r="P2" s="2">
+      <c r="P2" s="1">
         <v>26</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="Q2" s="1">
         <v>28</v>
       </c>
-      <c r="R2" s="2">
+      <c r="R2" s="1">
         <v>30</v>
       </c>
-      <c r="S2" s="2">
+      <c r="S2" s="1">
         <v>32</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="1">
         <v>34</v>
       </c>
-      <c r="U2" s="2">
+      <c r="U2" s="1">
         <v>36</v>
       </c>
-      <c r="V2" s="2">
+      <c r="V2" s="1">
         <v>38</v>
       </c>
-      <c r="W2" s="2">
+      <c r="W2" s="1">
         <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="7">
+      <c r="A3" s="5">
         <v>10</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="N3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="O3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="P3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="Q3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="R3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="S3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="T3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="U3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="V3" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="W3" s="4">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="N3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="O3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="P3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="R3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="S3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="T3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="U3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="V3" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="W3" s="3">
         <v>18808.2</v>
       </c>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="N4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="O4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="P4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="Q4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="R4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="S4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="T4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="U4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="V4" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="W4" s="4">
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="N4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="O4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="P4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="R4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="S4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="T4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="U4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="V4" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="W4" s="3">
         <v>18808.2</v>
       </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>13380</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>13818.9</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>14109.3</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>14190.3</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>14553.6</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>15159.3</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="3">
         <v>15300.6</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>15876.3</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="3">
         <v>16042.2</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <v>16538.099999999999</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="3">
         <v>17256</v>
       </c>
-      <c r="M5" s="4">
+      <c r="M5" s="3">
         <v>17917.2</v>
       </c>
-      <c r="N5" s="4">
+      <c r="N5" s="3">
         <v>18359.099999999999</v>
       </c>
-      <c r="O5" s="4">
+      <c r="O5" s="3">
         <v>18359.099999999999</v>
       </c>
-      <c r="P5" s="4">
+      <c r="P5" s="3">
         <v>18359.099999999999</v>
       </c>
-      <c r="Q5" s="4">
+      <c r="Q5" s="3">
         <v>18359.099999999999</v>
       </c>
-      <c r="R5" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="S5" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="T5" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="U5" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="V5" s="4">
-        <v>18808.2</v>
-      </c>
-      <c r="W5" s="4">
+      <c r="R5" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="S5" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="T5" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="U5" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="V5" s="3">
+        <v>18808.2</v>
+      </c>
+      <c r="W5" s="3">
         <v>18808.2</v>
       </c>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>11117.7</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>11634</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>11873.1</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>12063.6</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>12407.1</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>12747.3</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="3">
         <v>13140</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="3">
         <v>13531.5</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="3">
         <v>13925.1</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <v>15159.3</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="3">
         <v>16202.1</v>
       </c>
-      <c r="M6" s="4">
+      <c r="M6" s="3">
         <v>16202.1</v>
       </c>
-      <c r="N6" s="4">
+      <c r="N6" s="3">
         <v>16202.1</v>
       </c>
-      <c r="O6" s="4">
+      <c r="O6" s="3">
         <v>16202.1</v>
       </c>
-      <c r="P6" s="4">
+      <c r="P6" s="3">
         <v>16285.5</v>
       </c>
-      <c r="Q6" s="4">
+      <c r="Q6" s="3">
         <v>16285.5</v>
       </c>
-      <c r="R6" s="4">
+      <c r="R6" s="3">
         <v>16611</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="3">
         <v>16611</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="3">
         <v>16611</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="3">
         <v>16611</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="3">
         <v>16611</v>
       </c>
-      <c r="W6" s="4">
+      <c r="W6" s="3">
         <v>16611</v>
       </c>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="3">
         <v>8430.9</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>9261.9</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <v>9870</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>9870</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>9907.7999999999993</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>10332.299999999999</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>10388.700000000001</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="3">
         <v>10388.700000000001</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="3">
         <v>10979.1</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <v>12022.8</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="3">
         <v>12635.4</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="3">
         <v>13247.7</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="3">
         <v>13596.3</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="3">
         <v>13949.1</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="3">
         <v>14632.8</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="3">
         <v>14632.8</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="3">
         <v>14925</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="3">
         <v>14925</v>
       </c>
-      <c r="T7" s="4">
+      <c r="T7" s="3">
         <v>14925</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="3">
         <v>14925</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="3">
         <v>14925</v>
       </c>
-      <c r="W7" s="4">
+      <c r="W7" s="3">
         <v>14925</v>
       </c>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>7028.4</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>7917.3</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>8465.4</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>8568.6</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>8910.9</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>9114.9</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="3">
         <v>9564.9</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="3">
         <v>9895.7999999999993</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="3">
         <v>10322.700000000001</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <v>10974.3</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="3">
         <v>11285.1</v>
       </c>
-      <c r="M8" s="4">
+      <c r="M8" s="3">
         <v>11592.3</v>
       </c>
-      <c r="N8" s="4">
+      <c r="N8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="O8" s="4">
+      <c r="O8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="P8" s="4">
+      <c r="P8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="Q8" s="4">
+      <c r="Q8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="R8" s="4">
+      <c r="R8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="S8" s="4">
+      <c r="S8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="T8" s="4">
+      <c r="T8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8" s="3">
         <v>11940.9</v>
       </c>
-      <c r="W8" s="4">
+      <c r="W8" s="3">
         <v>11940.9</v>
       </c>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>6064.2</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>7019.7</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>7488.9</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>7592.4</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>8027.1</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>8493.6</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>9075</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="3">
         <v>9526.2000000000007</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="3">
         <v>9840.6</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <v>10020.9</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="3">
         <v>10125</v>
       </c>
-      <c r="M9" s="4">
+      <c r="M9" s="3">
         <v>10125</v>
       </c>
-      <c r="N9" s="4">
+      <c r="N9" s="3">
         <v>10125</v>
       </c>
-      <c r="O9" s="4">
+      <c r="O9" s="3">
         <v>10125</v>
       </c>
-      <c r="P9" s="4">
+      <c r="P9" s="3">
         <v>10125</v>
       </c>
-      <c r="Q9" s="4">
+      <c r="Q9" s="3">
         <v>10125</v>
       </c>
-      <c r="R9" s="4">
+      <c r="R9" s="3">
         <v>10125</v>
       </c>
-      <c r="S9" s="4">
+      <c r="S9" s="3">
         <v>10125</v>
       </c>
-      <c r="T9" s="4">
+      <c r="T9" s="3">
         <v>10125</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U9" s="3">
         <v>10125</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9" s="3">
         <v>10125</v>
       </c>
-      <c r="W9" s="4">
+      <c r="W9" s="3">
         <v>10125</v>
       </c>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>5331.6</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>6044.1</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>6522.6</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>7112.4</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>7453.8</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>7827.9</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="3">
         <v>8069.1</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="3">
         <v>8466.6</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="M10" s="4">
+      <c r="M10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="N10" s="4">
+      <c r="N10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="O10" s="4">
+      <c r="O10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="P10" s="4">
+      <c r="P10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="Q10" s="4">
+      <c r="Q10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="R10" s="4">
+      <c r="R10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="T10" s="4">
+      <c r="T10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10" s="3">
         <v>8674.5</v>
       </c>
-      <c r="W10" s="4">
+      <c r="W10" s="3">
         <v>8674.5</v>
       </c>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="3">
         <v>4606.8</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>5246.7</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>6042.9</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>6247.2</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="M11" s="4">
+      <c r="M11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="N11" s="4">
+      <c r="N11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="O11" s="4">
+      <c r="O11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="P11" s="4">
+      <c r="P11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="Q11" s="4">
+      <c r="Q11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="R11" s="4">
+      <c r="R11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="T11" s="4">
+      <c r="T11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V11" s="3">
         <v>6375.3</v>
       </c>
-      <c r="W11" s="4">
+      <c r="W11" s="3">
         <v>6375.3</v>
       </c>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>3998.4</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>4161.8999999999996</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="M12" s="4">
+      <c r="M12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="N12" s="4">
+      <c r="N12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="O12" s="4">
+      <c r="O12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="P12" s="4">
+      <c r="P12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="Q12" s="4">
+      <c r="Q12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="R12" s="4">
+      <c r="R12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="S12" s="4">
+      <c r="S12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="T12" s="4">
+      <c r="T12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="U12" s="4">
+      <c r="U12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="V12" s="4">
+      <c r="V12" s="3">
         <v>5031.3</v>
       </c>
-      <c r="W12" s="4">
+      <c r="W12" s="3">
         <v>5031.3</v>
       </c>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M13" s="4">
+      <c r="B13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" s="3">
         <v>9797.4</v>
       </c>
-      <c r="N13" s="4">
+      <c r="N13" s="3">
         <v>10294.5</v>
       </c>
-      <c r="O13" s="4">
+      <c r="O13" s="3">
         <v>10665</v>
       </c>
-      <c r="P13" s="4">
+      <c r="P13" s="3">
         <v>11074.2</v>
       </c>
-      <c r="Q13" s="4">
+      <c r="Q13" s="3">
         <v>11074.2</v>
       </c>
-      <c r="R13" s="4">
+      <c r="R13" s="3">
         <v>11628.9</v>
       </c>
-      <c r="S13" s="4">
+      <c r="S13" s="3">
         <v>11628.9</v>
       </c>
-      <c r="T13" s="4">
+      <c r="T13" s="3">
         <v>12209.4</v>
       </c>
-      <c r="U13" s="4">
+      <c r="U13" s="3">
         <v>12209.4</v>
       </c>
-      <c r="V13" s="4">
+      <c r="V13" s="3">
         <v>12821.1</v>
       </c>
-      <c r="W13" s="4">
+      <c r="W13" s="3">
         <v>12821.1</v>
       </c>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B14" s="3">
         <v>5510.4</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>5926.8</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>6096.9</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>6264.3</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>6552.9</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>6838.2</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="3">
         <v>7127.1</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>7560.9</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="3">
         <v>7941.9</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <v>8304.2999999999993</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="3">
         <v>8601.6</v>
       </c>
-      <c r="M14" s="4">
+      <c r="M14" s="3">
         <v>8891.1</v>
       </c>
-      <c r="N14" s="4">
+      <c r="N14" s="3">
         <v>9315.6</v>
       </c>
-      <c r="O14" s="4">
+      <c r="O14" s="3">
         <v>9664.7999999999993</v>
       </c>
-      <c r="P14" s="4">
+      <c r="P14" s="3">
         <v>10062.9</v>
       </c>
-      <c r="Q14" s="4">
+      <c r="Q14" s="3">
         <v>10062.9</v>
       </c>
-      <c r="R14" s="4">
+      <c r="R14" s="3">
         <v>10263.6</v>
       </c>
-      <c r="S14" s="4">
+      <c r="S14" s="3">
         <v>10263.6</v>
       </c>
-      <c r="T14" s="4">
+      <c r="T14" s="3">
         <v>10263.6</v>
       </c>
-      <c r="U14" s="4">
+      <c r="U14" s="3">
         <v>10263.6</v>
       </c>
-      <c r="V14" s="4">
+      <c r="V14" s="3">
         <v>10263.6</v>
       </c>
-      <c r="W14" s="4">
+      <c r="W14" s="3">
         <v>10263.6</v>
       </c>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="3">
         <v>5032.2</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>5241.3</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>5457</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>5526.9</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>5752.2</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>6195.6</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="3">
         <v>6657.6</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="3">
         <v>6875.1</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="3">
         <v>7126.8</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <v>7385.4</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="3">
         <v>7851.9</v>
       </c>
-      <c r="M15" s="4">
+      <c r="M15" s="3">
         <v>8166.3</v>
       </c>
-      <c r="N15" s="4">
+      <c r="N15" s="3">
         <v>8354.4</v>
       </c>
-      <c r="O15" s="4">
+      <c r="O15" s="3">
         <v>8554.5</v>
       </c>
-      <c r="P15" s="4">
+      <c r="P15" s="3">
         <v>8827.2000000000007</v>
       </c>
-      <c r="Q15" s="4">
+      <c r="Q15" s="3">
         <v>8827.2000000000007</v>
       </c>
-      <c r="R15" s="4">
+      <c r="R15" s="3">
         <v>8827.2000000000007</v>
       </c>
-      <c r="S15" s="4">
+      <c r="S15" s="3">
         <v>8827.2000000000007</v>
       </c>
-      <c r="T15" s="4">
+      <c r="T15" s="3">
         <v>8827.2000000000007</v>
       </c>
-      <c r="U15" s="4">
+      <c r="U15" s="3">
         <v>8827.2000000000007</v>
       </c>
-      <c r="V15" s="4">
+      <c r="V15" s="3">
         <v>8827.2000000000007</v>
       </c>
-      <c r="W15" s="4">
+      <c r="W15" s="3">
         <v>8827.2000000000007</v>
       </c>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="7" t="s">
+      <c r="A16" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B16" s="3">
         <v>4452.6000000000004</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>4873.8</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>5003.1000000000004</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>5092.5</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>5380.8</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>5829.6</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <v>6052.5</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>6271.2</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="3">
         <v>6539.1</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <v>6748.5</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="3">
         <v>6937.8</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="3">
         <v>7164.6</v>
       </c>
-      <c r="N16" s="4">
+      <c r="N16" s="3">
         <v>7313.7</v>
       </c>
-      <c r="O16" s="4">
+      <c r="O16" s="3">
         <v>7431.9</v>
       </c>
-      <c r="P16" s="4">
+      <c r="P16" s="3">
         <v>7431.9</v>
       </c>
-      <c r="Q16" s="4">
+      <c r="Q16" s="3">
         <v>7431.9</v>
       </c>
-      <c r="R16" s="4">
+      <c r="R16" s="3">
         <v>7431.9</v>
       </c>
-      <c r="S16" s="4">
+      <c r="S16" s="3">
         <v>7431.9</v>
       </c>
-      <c r="T16" s="4">
+      <c r="T16" s="3">
         <v>7431.9</v>
       </c>
-      <c r="U16" s="4">
+      <c r="U16" s="3">
         <v>7431.9</v>
       </c>
-      <c r="V16" s="4">
+      <c r="V16" s="3">
         <v>7431.9</v>
       </c>
-      <c r="W16" s="4">
+      <c r="W16" s="3">
         <v>7431.9</v>
       </c>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B17" s="3">
         <v>3908.1</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>4329.3</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>4442.1000000000004</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>4681.2</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>4963.5</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>5379.9</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="3">
         <v>5574.3</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>5847</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="3">
         <v>6114.3</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <v>6324.6</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="3">
         <v>6518.4</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="N17" s="4">
+      <c r="N17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="O17" s="4">
+      <c r="O17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="P17" s="4">
+      <c r="P17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="Q17" s="4">
+      <c r="Q17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="R17" s="4">
+      <c r="R17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="S17" s="4">
+      <c r="S17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="T17" s="4">
+      <c r="T17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="U17" s="4">
+      <c r="U17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="V17" s="4">
+      <c r="V17" s="3">
         <v>6753.6</v>
       </c>
-      <c r="W17" s="4">
+      <c r="W17" s="3">
         <v>6753.6</v>
       </c>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" s="5">
+      <c r="B18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H18" s="4">
         <v>6657.3</v>
       </c>
-      <c r="I18" s="5">
+      <c r="I18" s="4">
         <v>6807.9</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="4">
         <v>6997.8</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="4">
         <v>7221.6</v>
       </c>
-      <c r="L18" s="5">
+      <c r="L18" s="4">
         <v>7447.8</v>
       </c>
-      <c r="M18" s="5">
+      <c r="M18" s="4">
         <v>7808.4</v>
       </c>
-      <c r="N18" s="5">
+      <c r="N18" s="4">
         <v>8114.7</v>
       </c>
-      <c r="O18" s="5">
+      <c r="O18" s="4">
         <v>8436</v>
       </c>
-      <c r="P18" s="5">
+      <c r="P18" s="4">
         <v>8928.6</v>
       </c>
-      <c r="Q18" s="5">
+      <c r="Q18" s="4">
         <v>8928.6</v>
       </c>
-      <c r="R18" s="5">
+      <c r="R18" s="4">
         <v>9374.1</v>
       </c>
-      <c r="S18" s="5">
+      <c r="S18" s="4">
         <v>9374.1</v>
       </c>
-      <c r="T18" s="5">
+      <c r="T18" s="4">
         <v>9843.2999999999993</v>
       </c>
-      <c r="U18" s="5">
+      <c r="U18" s="4">
         <v>9843.2999999999993</v>
       </c>
-      <c r="V18" s="5">
+      <c r="V18" s="4">
         <v>10336.5</v>
       </c>
-      <c r="W18" s="5">
+      <c r="W18" s="4">
         <v>10336.5</v>
       </c>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G19" s="5">
+      <c r="B19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="4">
         <v>5449.5</v>
       </c>
-      <c r="H19" s="5">
+      <c r="H19" s="4">
         <v>5690.7</v>
       </c>
-      <c r="I19" s="5">
+      <c r="I19" s="4">
         <v>5839.8</v>
       </c>
-      <c r="J19" s="5">
+      <c r="J19" s="4">
         <v>6018.6</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="4">
         <v>6212.1</v>
       </c>
-      <c r="L19" s="5">
+      <c r="L19" s="4">
         <v>6561.9</v>
       </c>
-      <c r="M19" s="5">
+      <c r="M19" s="4">
         <v>6739.2</v>
       </c>
-      <c r="N19" s="5">
+      <c r="N19" s="4">
         <v>7040.7</v>
       </c>
-      <c r="O19" s="5">
+      <c r="O19" s="4">
         <v>7207.8</v>
       </c>
-      <c r="P19" s="5">
+      <c r="P19" s="4">
         <v>7619.4</v>
       </c>
-      <c r="Q19" s="5">
+      <c r="Q19" s="4">
         <v>7619.4</v>
       </c>
-      <c r="R19" s="5">
+      <c r="R19" s="4">
         <v>7772.1</v>
       </c>
-      <c r="S19" s="5">
+      <c r="S19" s="4">
         <v>7772.1</v>
       </c>
-      <c r="T19" s="5">
+      <c r="T19" s="4">
         <v>7772.1</v>
       </c>
-      <c r="U19" s="5">
+      <c r="U19" s="4">
         <v>7772.1</v>
       </c>
-      <c r="V19" s="5">
+      <c r="V19" s="4">
         <v>7772.1</v>
       </c>
-      <c r="W19" s="5">
+      <c r="W19" s="4">
         <v>7772.1</v>
       </c>
     </row>
     <row r="20" spans="1:23">
-      <c r="A20" s="7" t="s">
+      <c r="A20" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>3788.1</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>4134.3</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>4293</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>4502.1000000000004</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>4666.5</v>
       </c>
-      <c r="G20" s="5">
+      <c r="G20" s="4">
         <v>4947.6000000000004</v>
       </c>
-      <c r="H20" s="5">
+      <c r="H20" s="4">
         <v>5106.3</v>
       </c>
-      <c r="I20" s="5">
+      <c r="I20" s="4">
         <v>5387.1</v>
       </c>
-      <c r="J20" s="5">
+      <c r="J20" s="4">
         <v>5621.4</v>
       </c>
-      <c r="K20" s="5">
+      <c r="K20" s="4">
         <v>5781.3</v>
       </c>
-      <c r="L20" s="5">
+      <c r="L20" s="4">
         <v>5951.1</v>
       </c>
-      <c r="M20" s="5">
+      <c r="M20" s="4">
         <v>6017.1</v>
       </c>
-      <c r="N20" s="5">
+      <c r="N20" s="4">
         <v>6238.2</v>
       </c>
-      <c r="O20" s="5">
+      <c r="O20" s="4">
         <v>6356.7</v>
       </c>
-      <c r="P20" s="5">
+      <c r="P20" s="4">
         <v>6808.8</v>
       </c>
-      <c r="Q20" s="5">
+      <c r="Q20" s="4">
         <v>6808.8</v>
       </c>
-      <c r="R20" s="5">
+      <c r="R20" s="4">
         <v>6808.8</v>
       </c>
-      <c r="S20" s="5">
+      <c r="S20" s="4">
         <v>6808.8</v>
       </c>
-      <c r="T20" s="5">
+      <c r="T20" s="4">
         <v>6808.8</v>
       </c>
-      <c r="U20" s="5">
+      <c r="U20" s="4">
         <v>6808.8</v>
       </c>
-      <c r="V20" s="5">
+      <c r="V20" s="4">
         <v>6808.8</v>
       </c>
-      <c r="W20" s="5">
+      <c r="W20" s="4">
         <v>6808.8</v>
       </c>
     </row>
     <row r="21" spans="1:23">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>3276.6</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>3606</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>3765</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>3919.8</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>4080.6</v>
       </c>
-      <c r="G21" s="5">
+      <c r="G21" s="4">
         <v>4443.8999999999996</v>
       </c>
-      <c r="H21" s="5">
+      <c r="H21" s="4">
         <v>4585.2</v>
       </c>
-      <c r="I21" s="5">
+      <c r="I21" s="4">
         <v>4858.8</v>
       </c>
-      <c r="J21" s="5">
+      <c r="J21" s="4">
         <v>4942.5</v>
       </c>
-      <c r="K21" s="5">
+      <c r="K21" s="4">
         <v>5003.3999999999996</v>
       </c>
-      <c r="L21" s="5">
+      <c r="L21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="M21" s="5">
+      <c r="M21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="N21" s="5">
+      <c r="N21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="O21" s="5">
+      <c r="O21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="P21" s="5">
+      <c r="P21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="Q21" s="5">
+      <c r="Q21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="R21" s="5">
+      <c r="R21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="S21" s="5">
+      <c r="S21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="T21" s="5">
+      <c r="T21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="U21" s="5">
+      <c r="U21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="V21" s="5">
+      <c r="V21" s="4">
         <v>5074.8</v>
       </c>
-      <c r="W21" s="5">
+      <c r="W21" s="4">
         <v>5074.8</v>
       </c>
     </row>
     <row r="22" spans="1:23">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="4">
         <v>3220.5</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>3466.5</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>3637.5</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>3802.2</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>3959.4</v>
       </c>
-      <c r="G22" s="5">
+      <c r="G22" s="4">
         <v>4142.3999999999996</v>
       </c>
-      <c r="H22" s="5">
+      <c r="H22" s="4">
         <v>4234.5</v>
       </c>
-      <c r="I22" s="5">
+      <c r="I22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="J22" s="5">
+      <c r="J22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="K22" s="5">
+      <c r="K22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="L22" s="5">
+      <c r="L22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="N22" s="5">
+      <c r="N22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="O22" s="5">
+      <c r="O22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="P22" s="5">
+      <c r="P22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="Q22" s="5">
+      <c r="Q22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="R22" s="5">
+      <c r="R22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="S22" s="5">
+      <c r="S22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="T22" s="5">
+      <c r="T22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="U22" s="5">
+      <c r="U22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="V22" s="5">
+      <c r="V22" s="4">
         <v>4259.7</v>
       </c>
-      <c r="W22" s="5">
+      <c r="W22" s="4">
         <v>4259.7</v>
       </c>
     </row>
     <row r="23" spans="1:23">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>3027.3</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>3182.1</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>3354.9</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>3524.7</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="H23" s="5">
+      <c r="H23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="I23" s="5">
+      <c r="I23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="J23" s="5">
+      <c r="J23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="K23" s="5">
+      <c r="K23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="L23" s="5">
+      <c r="L23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="M23" s="5">
+      <c r="M23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="N23" s="5">
+      <c r="N23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="O23" s="5">
+      <c r="O23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="P23" s="5">
+      <c r="P23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="Q23" s="5">
+      <c r="Q23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="R23" s="5">
+      <c r="R23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="S23" s="5">
+      <c r="S23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="T23" s="5">
+      <c r="T23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="U23" s="5">
+      <c r="U23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="V23" s="5">
+      <c r="V23" s="4">
         <v>3675.6</v>
       </c>
-      <c r="W23" s="5">
+      <c r="W23" s="4">
         <v>3675.6</v>
       </c>
     </row>
     <row r="24" spans="1:23">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>2733</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>2904.6</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>3081</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>3081</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>3081</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="4">
         <v>3081</v>
       </c>
-      <c r="H24" s="5">
+      <c r="H24" s="4">
         <v>3081</v>
       </c>
-      <c r="I24" s="5">
+      <c r="I24" s="4">
         <v>3081</v>
       </c>
-      <c r="J24" s="5">
+      <c r="J24" s="4">
         <v>3081</v>
       </c>
-      <c r="K24" s="5">
+      <c r="K24" s="4">
         <v>3081</v>
       </c>
-      <c r="L24" s="5">
+      <c r="L24" s="4">
         <v>3081</v>
       </c>
-      <c r="M24" s="5">
+      <c r="M24" s="4">
         <v>3081</v>
       </c>
-      <c r="N24" s="5">
+      <c r="N24" s="4">
         <v>3081</v>
       </c>
-      <c r="O24" s="5">
+      <c r="O24" s="4">
         <v>3081</v>
       </c>
-      <c r="P24" s="5">
+      <c r="P24" s="4">
         <v>3081</v>
       </c>
-      <c r="Q24" s="5">
+      <c r="Q24" s="4">
         <v>3081</v>
       </c>
-      <c r="R24" s="5">
+      <c r="R24" s="4">
         <v>3081</v>
       </c>
-      <c r="S24" s="5">
+      <c r="S24" s="4">
         <v>3081</v>
       </c>
-      <c r="T24" s="5">
+      <c r="T24" s="4">
         <v>3081</v>
       </c>
-      <c r="U24" s="5">
+      <c r="U24" s="4">
         <v>3081</v>
       </c>
-      <c r="V24" s="5">
+      <c r="V24" s="4">
         <v>3081</v>
       </c>
-      <c r="W24" s="5">
+      <c r="W24" s="4">
         <v>3081</v>
       </c>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="M25" s="5">
+      <c r="M25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="O25" s="5">
+      <c r="O25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="P25" s="5">
+      <c r="P25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="Q25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="R25" s="5">
+      <c r="R25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="S25" s="5">
+      <c r="S25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="T25" s="5">
+      <c r="T25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="U25" s="5">
+      <c r="U25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="V25" s="5">
+      <c r="V25" s="4">
         <v>2599.1999999999998</v>
       </c>
-      <c r="W25" s="5">
+      <c r="W25" s="4">
         <v>2599.1999999999998</v>
       </c>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="7" t="s">
+      <c r="A26" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>2319</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="4">
         <v>2319</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="4">
         <v>2319</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="4">
         <v>2319</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>2319</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="4">
         <v>2319</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H26" s="4">
         <v>2319</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I26" s="4">
         <v>2319</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J26" s="4">
         <v>2319</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K26" s="4">
         <v>2319</v>
       </c>
-      <c r="L26" s="5">
+      <c r="L26" s="4">
         <v>2319</v>
       </c>
-      <c r="M26" s="5">
+      <c r="M26" s="4">
         <v>2319</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N26" s="4">
         <v>2319</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O26" s="4">
         <v>2319</v>
       </c>
-      <c r="P26" s="5">
+      <c r="P26" s="4">
         <v>2319</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="Q26" s="4">
         <v>2319</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R26" s="4">
         <v>2319</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S26" s="4">
         <v>2319</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T26" s="4">
         <v>2319</v>
       </c>
-      <c r="U26" s="5">
+      <c r="U26" s="4">
         <v>2319</v>
       </c>
-      <c r="V26" s="5">
+      <c r="V26" s="4">
         <v>2319</v>
       </c>
-      <c r="W26" s="5">
+      <c r="W26" s="4">
         <v>2319</v>
       </c>
     </row>

</xml_diff>